<commit_message>
logica terminada al 80%
</commit_message>
<xml_diff>
--- a/registro_entradas/2024-12-20.xlsx
+++ b/registro_entradas/2024-12-20.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,10 +439,15 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>TOKENS</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>FECHA</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>HORA</t>
         </is>
@@ -454,22 +459,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Andres Salcedo</t>
+          <t>andres salcedo</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sistemas</t>
+          <t>sistemas</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>2024-12-20</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>15:02:41</t>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>16:04:15</t>
         </is>
       </c>
     </row>

</xml_diff>